<commit_message>
changing float to number
our column b was scientific
</commit_message>
<xml_diff>
--- a/default/ValueMeas.xlsx
+++ b/default/ValueMeas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odinn.h\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\KOP-File\FjarmalOgStjorn_Notendur$\odinn.h\My Documents\GitHub\EntityFiles\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C61575-249E-4A45-80A4-16330A654C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9209E3B1-C89A-4587-8BB3-6AB15AC43F9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64890" yWindow="1200" windowWidth="14040" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -77,7 +77,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,7 +361,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,11 +383,9 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
       <c r="C2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
       <c r="C3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>